<commit_message>
Test Scripts of Resume Builder
</commit_message>
<xml_diff>
--- a/Resume_Builder_Framework/src/test/resources/TestData/testData.xlsx
+++ b/Resume_Builder_Framework/src/test/resources/TestData/testData.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="4740" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="kjhuhuh" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,13 +22,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Likhithavgowda</t>
+  </si>
+  <si>
+    <t>rfrhhthm</t>
+  </si>
+  <si>
+    <t>likhitha</t>
+  </si>
+  <si>
+    <t>vjkggvnb</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -53,8 +77,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,12 +363,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:A7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.109375" customWidth="1"/>
+    <col min="3" max="3" width="43.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>